<commit_message>
Update with working exercise for RM meeting
</commit_message>
<xml_diff>
--- a/exercise/hfc_inputs.xlsx
+++ b/exercise/hfc_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>variable</t>
   </si>
@@ -57,9 +57,6 @@
     <t>consent_value</t>
   </si>
   <si>
-    <t>consent</t>
-  </si>
-  <si>
     <t>specify_variable</t>
   </si>
   <si>
@@ -69,94 +66,13 @@
     <t>iqr_multiplier</t>
   </si>
   <si>
-    <t>gpsLatitude</t>
-  </si>
-  <si>
-    <t>gpsLongitude</t>
-  </si>
-  <si>
-    <t>SubmissionDate</t>
-  </si>
-  <si>
-    <t>starttime</t>
-  </si>
-  <si>
-    <t>endtime</t>
-  </si>
-  <si>
-    <t>deviceid</t>
-  </si>
-  <si>
-    <t>audit_data</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>ward</t>
-  </si>
-  <si>
-    <t>literacy</t>
-  </si>
-  <si>
-    <t>consentsign</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>language_other</t>
-  </si>
-  <si>
-    <t>edustatus</t>
-  </si>
-  <si>
-    <t>eduattain</t>
-  </si>
-  <si>
-    <t>employmt</t>
-  </si>
-  <si>
-    <t>employyear</t>
-  </si>
-  <si>
-    <t>occupation</t>
-  </si>
-  <si>
-    <t>occupation_other</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>relationship</t>
-  </si>
-  <si>
-    <t>childnum</t>
-  </si>
-  <si>
-    <t>finalnotes</t>
-  </si>
-  <si>
-    <t>intstatus</t>
-  </si>
-  <si>
-    <t>intstatus_other</t>
-  </si>
-  <si>
     <t>submission_date</t>
-  </si>
-  <si>
-    <t>ta_*</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
     <t>other_unique</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
   <si>
     <t>assert</t>
@@ -189,46 +105,7 @@
     <t>days</t>
   </si>
   <si>
-    <t>enumid</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>pregnant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employyear </t>
-  </si>
-  <si>
-    <t>supid</t>
-  </si>
-  <si>
-    <t>instatus</t>
-  </si>
-  <si>
     <t>if_condition</t>
-  </si>
-  <si>
-    <t>pregnant==.</t>
-  </si>
-  <si>
-    <t>gender==0</t>
-  </si>
-  <si>
-    <t>salary==.</t>
-  </si>
-  <si>
-    <t>employmt==0</t>
-  </si>
-  <si>
-    <t>occupation==.</t>
-  </si>
-  <si>
-    <t>employyear==4</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +910,1019 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="314325"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="47625"/>
+          <a:ext cx="3648075" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>HFC Check #</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t> 10</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Check date</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> variables.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This check verifies that:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    1. survey start and end dates are unmissing</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    2. survey start and end dates are equal</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    3. survey start dates are not before start of data collection</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    4. survey start dates are not after the current date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    5. survey start dates within the same geographic cluster </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>        are within X days of each other (OPTIONAL).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="1971675"/>
+          <a:ext cx="3667125" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>startdate</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the variable containing the survey start date. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="2686050"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enddate</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This column specifies the variable containing the survey end date. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="3381375"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>surveystart</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This column specifies the variable containing date that data collection began.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="4076700"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>enum</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>area</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the variable representing geographic clusters.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="4772025"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>days</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the number of days to that surveys within the same cluster should fall within</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9715500" y="5476875"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>output_variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9715500" y="6172200"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13954125" y="590550"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="TextBox 12"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Rectangle 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle 14"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1429,10 +2315,179 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="361950"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1882,6 +2937,175 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="12582525" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2285,6 +3509,175 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="323850"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="TextBox 2"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2679,6 +4072,175 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="304800"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="TextBox 12"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Rectangle 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle 14"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3003,10 +4565,687 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8439150" y="304800"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="47625"/>
+          <a:ext cx="3648075" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>HFC Check # 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Check that follow up record</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>s match master</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This check applies to follow up or post-census surveys. It checks relevant identification variables against a master tracking list to ensure the data are matching. The name of the master list is specified in the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>master_check.do </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>file. Note, that you must have </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>cfout</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> installed for this check to work properly.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="1790701"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>variable</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the names of the variables to check for matches in the master and follow up.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="2476500"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>output_variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="3181350"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8429625" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3467,10 +5706,179 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11201400" y="381000"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3791,10 +6199,179 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1228725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8420100" y="600075"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4439,10 +7016,179 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Group 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13954125" y="581025"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="TextBox 10"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Rectangle 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4765,675 +7511,173 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8334375" y="47625"/>
-          <a:ext cx="3648075" cy="1828800"/>
+          <a:off x="8429625" y="695325"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
-            <a:t>HFC Check #</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
-            <a:t> 10</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Check date</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> variables.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies that:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    1. survey start and end dates are unmissing</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    2. survey start and end dates are equal</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    3. survey start dates are not before start of data collection</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    4. survey start dates are not after the current date</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    5. survey start dates within the same geographic cluster </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>        are within X days of each other (OPTIONAL).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="1971675"/>
-          <a:ext cx="3667125" cy="647700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
               <a:shade val="50000"/>
             </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>startdate</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the variable containing the survey start date. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="2686050"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
               <a:shade val="50000"/>
             </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enddate</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This column specifies the variable containing the survey end date. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="3381375"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>surveystart</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This column specifies the variable containing date that data collection began.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="4076700"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>enum</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>area</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the variable representing geographic clusters.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="4772025"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>days</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the number of days to that surveys within the same cluster should fall within</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9715500" y="5476875"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9715500" y="6172200"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5704,8 +7948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -5718,21 +7962,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5759,7 +7995,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -5772,31 +8008,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4">
-        <v>42309</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -5833,7 +8062,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -5843,33 +8072,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="6">
-        <v>3</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5899,91 +8119,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3"/>
@@ -6189,7 +8376,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -6202,7 +8389,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6212,19 +8399,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3"/>
@@ -6250,7 +8435,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6263,27 +8448,14 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
+      <c r="A3" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
@@ -6306,7 +8478,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A10" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6316,65 +8488,41 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="A10" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
@@ -6394,52 +8542,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3">
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:3">
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1">
+  <conditionalFormatting sqref="A1:C1">
     <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6448,7 +8591,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6458,65 +8601,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="E5" s="3"/>
     </row>
   </sheetData>
@@ -6539,8 +8656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C602"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6550,176 +8667,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
       <c r="C32" s="3"/>
     </row>
     <row r="34" spans="1:3">
@@ -7313,7 +9297,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -7335,47 +9319,23 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>10000</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="3"/>
@@ -7851,32 +9811,28 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="5" spans="1:3">

</xml_diff>